<commit_message>
2.1.1: using apache poi v4.1.2.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoAntTaskConstants.xlsx
+++ b/meta/program/BlancoAntTaskConstants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoAntTask/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEBADE5B-F7A4-D547-B9D8-CE32481424EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C3ACED-FEF8-874B-905B-403DA1079488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="640"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -136,9 +136,6 @@
     <t>VERSION</t>
   </si>
   <si>
-    <t>"0.7.5"</t>
-  </si>
-  <si>
     <t>バージョン番号。</t>
   </si>
   <si>
@@ -155,12 +152,16 @@
   </si>
   <si>
     <t>○</t>
+  </si>
+  <si>
+    <t>"2.1.1"</t>
+    <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -1004,7 +1005,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1250,10 +1251,10 @@
         <v>25</v>
       </c>
       <c r="D22" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="26" t="s">
         <v>32</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>33</v>
       </c>
       <c r="F22" s="30"/>
       <c r="G22"/>
@@ -1264,16 +1265,16 @@
         <v>4</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="26" t="s">
         <v>35</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>36</v>
       </c>
       <c r="F23" s="30"/>
       <c r="G23"/>
@@ -1377,19 +1378,19 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D47">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D47" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustConstValue</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>isAbstract</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>accessScope</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1403,7 +1404,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1423,7 +1424,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1458,10 +1459,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:10">

</xml_diff>